<commit_message>
kNN mix up and running.
</commit_message>
<xml_diff>
--- a/AutomatedNeuralNetwork/draftOneGraphs - fix me.xlsx
+++ b/AutomatedNeuralNetwork/draftOneGraphs - fix me.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>Diabetes</t>
   </si>
@@ -38,10 +38,10 @@
     <t>Accuracy</t>
   </si>
   <si>
-    <t>2 Layers</t>
+    <t>3 Layers (LR .1)</t>
   </si>
   <si>
-    <t>3 Layers</t>
+    <t>2 Layers (LR .1)</t>
   </si>
 </sst>
 </file>
@@ -167,21 +167,23 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -234,7 +236,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>2 Layers</a:t>
+              <a:t>2 Layers (LR .1)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -376,11 +378,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="239108352"/>
-        <c:axId val="239109472"/>
+        <c:axId val="142467136"/>
+        <c:axId val="142467696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="239108352"/>
+        <c:axId val="142467136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -437,12 +439,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239109472"/>
+        <c:crossAx val="142467696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="239109472"/>
+        <c:axId val="142467696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -499,7 +501,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239108352"/>
+        <c:crossAx val="142467136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -660,33 +662,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3000</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -696,33 +671,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>66.666700000000006</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>84.444400000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>86.666700000000006</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>75.555599999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>75.666600000000003</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>77.777799999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>66.666700000000006</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>86.666700000000006</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>82.222200000000001</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -736,11 +684,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="182068448"/>
-        <c:axId val="237331216"/>
+        <c:axId val="142469936"/>
+        <c:axId val="142470496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="182068448"/>
+        <c:axId val="142469936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -797,12 +745,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237331216"/>
+        <c:crossAx val="142470496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="237331216"/>
+        <c:axId val="142470496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -859,7 +807,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="182068448"/>
+        <c:crossAx val="142469936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -904,6 +852,360 @@
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>3</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Layers (LR .1)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>350</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$4:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>68.695700000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.695700000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70.869600000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69.658199999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>71.348299999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="217199472"/>
+        <c:axId val="217198912"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="217199472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="217198912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="217198912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="217199472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -988,6 +1290,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1505,6 +1847,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2077,6 +2935,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2350,417 +3238,411 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="9" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="1">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="2">
         <v>71.739099999999993</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="1">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>68.695700000000002</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="1">
         <v>50</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>72.173900000000003</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="1">
+        <v>50</v>
+      </c>
+      <c r="E5" s="2">
+        <v>68.695700000000002</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="1">
         <v>100</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="2">
         <v>70.869600000000005</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="1">
+        <v>100</v>
+      </c>
+      <c r="E6" s="2">
+        <v>70.869600000000005</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="1">
         <v>150</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="2">
         <v>69.130399999999995</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="1">
+        <v>150</v>
+      </c>
+      <c r="E7" s="2">
+        <v>69.658199999999994</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="1">
         <v>200</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="2">
         <v>71.739099999999993</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="1">
+        <v>200</v>
+      </c>
+      <c r="E8" s="2">
+        <v>71.348299999999995</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="1">
         <v>250</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="2">
         <v>70.869600000000005</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="1">
+        <v>250</v>
+      </c>
+      <c r="E9" s="2">
+        <v>70</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="1">
         <v>300</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="2">
         <v>70</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="1">
+        <v>300</v>
+      </c>
+      <c r="E10" s="2">
+        <v>71</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11" s="3">
         <v>350</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <v>67.826099999999997</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="3">
+        <v>350</v>
+      </c>
+      <c r="E11" s="4">
+        <v>72</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J12" s="11"/>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9" t="s">
+      <c r="A13" s="5"/>
+      <c r="B13" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="1" t="s">
+      <c r="C14" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="C15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="D15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="C16" s="1">
         <v>5</v>
       </c>
-      <c r="B16" s="4">
+      <c r="D16" s="2">
         <v>66.666700000000006</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="C17" s="1">
         <v>50</v>
       </c>
-      <c r="B17" s="4">
+      <c r="D17" s="2">
         <v>84.444400000000002</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="C18" s="1">
         <v>100</v>
       </c>
-      <c r="B18" s="4">
+      <c r="D18" s="2">
         <v>86.666700000000006</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="C19" s="1">
         <v>150</v>
       </c>
-      <c r="B19" s="4">
+      <c r="D19" s="2">
         <v>75.555599999999998</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="C20" s="1">
         <v>200</v>
       </c>
-      <c r="B20" s="4">
+      <c r="D20" s="2">
         <v>75.666600000000003</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="C21" s="1">
         <v>1500</v>
       </c>
-      <c r="B21" s="4">
+      <c r="D21" s="2">
         <v>77.777799999999999</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="C22" s="1">
         <v>2000</v>
       </c>
-      <c r="B22" s="4">
+      <c r="D22" s="2">
         <v>66.666700000000006</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="C23" s="1">
         <v>2500</v>
       </c>
-      <c r="B23" s="4">
+      <c r="D23" s="2">
         <v>86.666700000000006</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
+      <c r="C24" s="3">
         <v>3000</v>
       </c>
-      <c r="B24" s="6">
+      <c r="D24" s="4">
         <v>82.222200000000001</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
+      <c r="A26" s="3"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A14:B14"/>
+  <mergeCells count="5">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>